<commit_message>
fix issue 6174 y 6175
</commit_message>
<xml_diff>
--- a/src/assets/files/10.GruposProgramas O ProgramasTrabajoSocial.xlsx
+++ b/src/assets/files/10.GruposProgramas O ProgramasTrabajoSocial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brquezada\Documents\projects\frontEnd\gui-mst-adt-web\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avictoria\Documents\Proyectos\AgendaDigital\ARCHIVOS PRUEBA\oficiales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEA1522-B77C-46F9-8F5F-01D7A15D775F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F16279E-B6D1-4D99-AD8C-2AEA5C756757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{A368C07F-A6F7-4CCA-94AA-ED26F8537688}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="21756" windowHeight="10836" activeTab="1" xr2:uid="{A368C07F-A6F7-4CCA-94AA-ED26F8537688}"/>
   </bookViews>
   <sheets>
     <sheet name="A_servicios_especialidades" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>CLAVE ESPECIALIDAD</t>
   </si>
@@ -77,15 +77,6 @@
     <t>AC01</t>
   </si>
   <si>
-    <t xml:space="preserve">Atención Médica Continúa </t>
-  </si>
-  <si>
-    <t>Tabaquismo</t>
-  </si>
-  <si>
-    <t>CLAVE GRUPO</t>
-  </si>
-  <si>
     <t>DESCRIPCION GRUPO / PROGRAMA</t>
   </si>
   <si>
@@ -98,13 +89,10 @@
     <t>SERVICIO/ESPECIALIDAD</t>
   </si>
   <si>
-    <t>Tour  Quirúrgico</t>
-  </si>
-  <si>
-    <t>TS2.C</t>
-  </si>
-  <si>
-    <t>Tour Quirúrgico</t>
+    <t>Trabajo Social</t>
+  </si>
+  <si>
+    <t>VIH</t>
   </si>
 </sst>
 </file>
@@ -460,15 +448,15 @@
   <dimension ref="A1:L195"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.36328125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,12 +494,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>12</v>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -535,25 +523,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J30" s="1"/>
     </row>
-    <row r="46" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J47" s="1"/>
     </row>
-    <row r="56" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J56" s="1"/>
     </row>
-    <row r="69" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J69" s="1"/>
     </row>
-    <row r="194" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="194" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K194" s="1"/>
     </row>
-    <row r="195" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="195" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K195" s="1"/>
     </row>
   </sheetData>
@@ -563,52 +551,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6906E3C9-43FF-4585-8045-F2045195D951}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="2" max="2" width="34.81640625" customWidth="1"/>
-    <col min="4" max="4" width="41.90625" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="1" max="1" width="34.77734375" customWidth="1"/>
+    <col min="3" max="3" width="41.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -732,18 +713,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -763,18 +744,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D190155-82FD-4E67-B123-72C736F412C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{993EAD62-0B42-413E-BEAB-9130C6195D77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D190155-82FD-4E67-B123-72C736F412C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix carga masiva programa 6174
</commit_message>
<xml_diff>
--- a/src/assets/files/10.GruposProgramas O ProgramasTrabajoSocial.xlsx
+++ b/src/assets/files/10.GruposProgramas O ProgramasTrabajoSocial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avictoria\Documents\Proyectos\AgendaDigital\ARCHIVOS PRUEBA\oficiales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F16279E-B6D1-4D99-AD8C-2AEA5C756757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3168A04D-E6F3-43B2-9DBD-2B565B773B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="21756" windowHeight="10836" activeTab="1" xr2:uid="{A368C07F-A6F7-4CCA-94AA-ED26F8537688}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>CLAVE ESPECIALIDAD</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>VIH</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -128,9 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,20 +555,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6906E3C9-43FF-4585-8045-F2045195D951}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.77734375" customWidth="1"/>
     <col min="3" max="3" width="41.88671875" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -574,11 +579,14 @@
       <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -588,7 +596,10 @@
       <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -599,6 +610,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002047D94B5E73D04A80AA6844A59F543A" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="19f8b377e75dbac3c1f2314aec064948">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f6edc329ff236629c56e3b879b320d0">
     <xsd:element name="properties">
@@ -712,15 +732,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -728,6 +739,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D190155-82FD-4E67-B123-72C736F412C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6D1E4D6-D892-4D9D-A66D-7D06C6047DED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -743,14 +762,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D190155-82FD-4E67-B123-72C736F412C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{993EAD62-0B42-413E-BEAB-9130C6195D77}">
   <ds:schemaRefs>

</xml_diff>